<commit_message>
add training code and update new data
</commit_message>
<xml_diff>
--- a/data/raw_data_restore_uppercase.xlsx
+++ b/data/raw_data_restore_uppercase.xlsx
@@ -4487,7 +4487,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>[('41', '54', 'PROPERTY'), ('55', '66', 'PROPERTY'), ('153', '157', 'MAT'), ('295', '299', 'MAT'), ('357', '363', 'WEIGHT'), ('11', '25', 'PROPERTY'), ('84', '103', 'PROPERTY'), ('232', '240', 'SHAPE'), ('189', '223', 'DIMENSION'), ('302', '310', 'PROPERTY'), ('313', '324', 'PROPERTY')]</t>
+          <t>[('41', '54', 'PROPERTY'), ('55', '66', 'PROPERTY'), ('153', '157', 'COLOR'), ('295', '299', 'MAT'), ('357', '363', 'WEIGHT'), ('11', '25', 'PROPERTY'), ('84', '103', 'PROPERTY'), ('232', '240', 'SHAPE'), ('189', '223', 'DIMENSION'), ('302', '310', 'PROPERTY'), ('313', '324', 'PROPERTY')]</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -8057,7 +8057,7 @@
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>[('41', '54', 'PROPERTY'), ('55', '66', 'PROPERTY'), ('153', '157', 'MAT'), ('295', '299', 'MAT'), ('357', '363', 'WEIGHT'), ('11', '25', 'PROPERTY'), ('84', '103', 'PROPERTY'), ('108', '120', 'PROPERTY'), ('232', '240', 'SHAPE'), ('189', '223', 'DIMENSION'), ('302', '310', 'PROPERTY'), ('313', '324', 'PROPERTY')]</t>
+          <t>[('41', '54', 'PROPERTY'), ('55', '66', 'PROPERTY'), ('153', '157', 'COLOR'), ('295', '299', 'MAT'), ('357', '363', 'WEIGHT'), ('11', '25', 'PROPERTY'), ('84', '103', 'PROPERTY'), ('108', '120', 'PROPERTY'), ('232', '240', 'SHAPE'), ('189', '223', 'DIMENSION'), ('302', '310', 'PROPERTY'), ('313', '324', 'PROPERTY')]</t>
         </is>
       </c>
       <c r="C449" t="inlineStr">
@@ -27165,12 +27165,12 @@
       </c>
       <c r="B1573" t="inlineStr">
         <is>
-          <t>[('18', '27', 'PROPERTY'), ('32', '38', 'PROPERTY'), ('44', '59', 'PROPERTY'), ('116', '125', 'MAIN_PRODUCT'), ('132', '142', 'PROPERTY'), ('143', '149', 'MAT')]</t>
+          <t>[('18', '27', 'PROPERTY'), ('32', '38', 'PROPERTY'), ('44', '59', 'PROPERTY'), ('132', '142', 'PROPERTY'), ('143', '149', 'MAT')]</t>
         </is>
       </c>
       <c r="C1573" t="inlineStr">
         <is>
-          <t>['four legs', 'welded', 'x - shaped rods', 'table leg', 'non - slip', 'rubber']</t>
+          <t>['four legs', 'welded', 'x - shaped rods', 'non - slip', 'rubber']</t>
         </is>
       </c>
     </row>

</xml_diff>